<commit_message>
Updated to 2021-01-13; XLSX data export improved;
</commit_message>
<xml_diff>
--- a/data/xlsx/data.01.xlsx
+++ b/data/xlsx/data.01.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5984" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6001" uniqueCount="353">
   <si>
     <t>TIME</t>
   </si>
@@ -1085,6 +1085,9 @@
   <si>
     <t>2021-01-12 11:00:00</t>
   </si>
+  <si>
+    <t>2021-01-13 11:00:00</t>
+  </si>
 </sst>
 </file>
 
@@ -6020,6 +6023,20 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -10919,6 +10936,20 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -15818,6 +15849,20 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -20717,6 +20762,20 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>187.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -25616,6 +25675,20 @@
         <v>9.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>289.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>390.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -30515,6 +30588,20 @@
         <v>4.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>228.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>252.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -35414,6 +35501,20 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -40313,6 +40414,20 @@
         <v>11.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -45212,6 +45327,20 @@
         <v>8.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>213.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>468.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -50111,6 +50240,20 @@
         <v>8.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>199.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -55010,6 +55153,20 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -59909,6 +60066,20 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -64808,6 +64979,20 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>239.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>271.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -69707,6 +69892,20 @@
         <v>4.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>168.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -74606,6 +74805,20 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>167.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>149.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -79505,6 +79718,20 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>179.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>261.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -84404,6 +84631,20 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>352</v>
+      </c>
+      <c r="B350" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C350" t="n">
+        <v>144.0</v>
+      </c>
+      <c r="D350" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>